<commit_message>
Get Student List Rest Operation development
</commit_message>
<xml_diff>
--- a/TaskLists.xlsx
+++ b/TaskLists.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Task</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>4d</t>
+  </si>
+  <si>
+    <t>Student find rest operation developments as a student id  If you don't find any record with this student number. you have to throw custom error object.. getStudent(id)</t>
+  </si>
+  <si>
+    <t>Student update rest operation developments as a student If you don't find any record with this student number. you have to throw custom error object.. (put(id)</t>
+  </si>
+  <si>
+    <t>Student update rest operation developments as a student If you don't find any record with this student number. you have to throw custom error object.. PATCH(id)</t>
   </si>
 </sst>
 </file>
@@ -319,156 +328,187 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599990"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399980"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -478,7 +518,9 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
@@ -493,33 +535,25 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -534,9 +568,7 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -551,9 +583,7 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -568,17 +598,13 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <top style="thin">
@@ -587,9 +613,7 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal style="none">
-        <color rgb="FF000000"/>
-      </diagonal>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -604,7 +628,9 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -1008,7 +1034,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.200000"/>
@@ -1155,7 +1181,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>30</v>
@@ -1182,7 +1208,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>26</v>
@@ -1209,7 +1235,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>30</v>

</xml_diff>